<commit_message>
Exámenes Ordinario/Extraordinario - 30 Mayo 2024 - Lap HP
Se actualiza el repositorio con los exámenes ordinarios (primera y segunda vuelta) así como el examen extraordinario de Física 4 (Área II)
</commit_message>
<xml_diff>
--- a/Bitacoras/Concentrado_Grupo_93.xlsx
+++ b/Bitacoras/Concentrado_Grupo_93.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_4\Bitacoras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BED63B-4A6A-49CB-8801-5A8D15297D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F876BC9F-9BC7-4F12-9996-A834CB241506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CC7B38A6-024E-4FE0-910A-92260C6A95BF}"/>
   </bookViews>
@@ -838,10 +838,10 @@
   <dimension ref="A1:AD14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="6900" ySplit="1155" topLeftCell="P2" activePane="bottomRight"/>
+      <pane xSplit="6900" ySplit="1155" topLeftCell="T2" activePane="bottomRight"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
-      <selection pane="bottomRight" activeCell="W14" sqref="W14"/>
+      <selection pane="bottomRight" activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>